<commit_message>
added script to print labels
</commit_message>
<xml_diff>
--- a/data/planning.xlsx
+++ b/data/planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pth7\Documents\Intercrop JLJ\2025_winter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265139E4-B59A-47C7-BE99-D9C0D3DD7D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429F118B-F67E-4592-83FB-2A049019571E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{BEFE39CF-4712-4775-9411-5C503787578E}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{BEFE39CF-4712-4775-9411-5C503787578E}"/>
   </bookViews>
   <sheets>
     <sheet name="selections" sheetId="1" r:id="rId1"/>
@@ -656,9 +656,6 @@
     <t>&lt;</t>
   </si>
   <si>
-    <t>Winter Oat/Pea Trial (M XM)</t>
-  </si>
-  <si>
     <t>Heading - %|CO_350:0005127</t>
   </si>
   <si>
@@ -999,6 +996,9 @@
   </si>
   <si>
     <t>replicates</t>
+  </si>
+  <si>
+    <t>Winter Oat/Pea Trial (66M X 45M)</t>
   </si>
 </sst>
 </file>
@@ -1606,7 +1606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E147DB-166A-44B5-BCC5-098A0311CA8B}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
@@ -1625,7 +1625,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1640,13 +1640,13 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1654,7 +1654,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -1680,7 +1680,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1706,7 +1706,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -1732,7 +1732,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -1758,7 +1758,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -1784,7 +1784,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -1810,7 +1810,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -1836,7 +1836,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
@@ -1862,7 +1862,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C10" t="s">
         <v>32</v>
@@ -1888,7 +1888,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C11" t="s">
         <v>40</v>
@@ -1914,7 +1914,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -1940,7 +1940,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
@@ -1966,7 +1966,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
@@ -1992,7 +1992,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
@@ -2018,7 +2018,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
@@ -2044,7 +2044,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -2070,7 +2070,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C18" t="s">
         <v>44</v>
@@ -2096,7 +2096,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
@@ -2122,7 +2122,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C20" t="s">
         <v>46</v>
@@ -2148,7 +2148,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C21" t="s">
         <v>30</v>
@@ -2174,7 +2174,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C22" t="s">
         <v>28</v>
@@ -2200,7 +2200,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C23" t="s">
         <v>70</v>
@@ -2226,7 +2226,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C24" t="s">
         <v>52</v>
@@ -2252,7 +2252,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C25" t="s">
         <v>48</v>
@@ -2278,7 +2278,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C26" t="s">
         <v>56</v>
@@ -2304,7 +2304,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C27" t="s">
         <v>68</v>
@@ -2330,7 +2330,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C28" t="s">
         <v>50</v>
@@ -2356,7 +2356,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C29" t="s">
         <v>62</v>
@@ -2382,7 +2382,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C30" t="s">
         <v>58</v>
@@ -2408,7 +2408,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C31" t="s">
         <v>54</v>
@@ -2434,7 +2434,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C32" t="s">
         <v>80</v>
@@ -2460,7 +2460,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C33" t="s">
         <v>72</v>
@@ -2486,7 +2486,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C34" t="s">
         <v>92</v>
@@ -2512,7 +2512,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C35" t="s">
         <v>96</v>
@@ -2538,7 +2538,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C36" t="s">
         <v>86</v>
@@ -2564,7 +2564,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C37" t="s">
         <v>60</v>
@@ -2590,7 +2590,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C38" t="s">
         <v>84</v>
@@ -2616,7 +2616,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C39" t="s">
         <v>66</v>
@@ -2642,7 +2642,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C40" t="s">
         <v>76</v>
@@ -2668,7 +2668,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C41" t="s">
         <v>42</v>
@@ -2694,7 +2694,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C42" t="s">
         <v>112</v>
@@ -2720,7 +2720,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C43" t="s">
         <v>74</v>
@@ -2746,7 +2746,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C44" t="s">
         <v>90</v>
@@ -2772,7 +2772,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C45" t="s">
         <v>82</v>
@@ -2798,7 +2798,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C46" t="s">
         <v>114</v>
@@ -2824,7 +2824,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C47" t="s">
         <v>98</v>
@@ -2850,7 +2850,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C48" t="s">
         <v>118</v>
@@ -2876,7 +2876,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C49" t="s">
         <v>106</v>
@@ -2902,7 +2902,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C50" t="s">
         <v>64</v>
@@ -2928,7 +2928,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C51" t="s">
         <v>88</v>
@@ -2954,7 +2954,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C52" t="s">
         <v>100</v>
@@ -2980,7 +2980,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C53" t="s">
         <v>126</v>
@@ -3006,7 +3006,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C54" t="s">
         <v>94</v>
@@ -3032,7 +3032,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C55" t="s">
         <v>122</v>
@@ -3058,7 +3058,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C56" t="s">
         <v>104</v>
@@ -3084,7 +3084,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C57" t="s">
         <v>110</v>
@@ -3110,7 +3110,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C58" t="s">
         <v>124</v>
@@ -3136,7 +3136,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C59" t="s">
         <v>120</v>
@@ -3162,7 +3162,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C60" t="s">
         <v>102</v>
@@ -3188,7 +3188,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C61" t="s">
         <v>78</v>
@@ -3214,7 +3214,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C62" t="s">
         <v>130</v>
@@ -3240,7 +3240,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C63" t="s">
         <v>108</v>
@@ -3266,13 +3266,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C64" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D64" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E64">
         <v>948</v>
@@ -3292,7 +3292,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C65" t="s">
         <v>136</v>
@@ -3318,7 +3318,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C66" t="s">
         <v>128</v>
@@ -3344,7 +3344,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C67" t="s">
         <v>140</v>
@@ -3370,7 +3370,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C68" t="s">
         <v>116</v>
@@ -3396,13 +3396,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C69" t="s">
+        <v>313</v>
+      </c>
+      <c r="D69" t="s">
         <v>314</v>
-      </c>
-      <c r="D69" t="s">
-        <v>315</v>
       </c>
       <c r="E69">
         <v>793</v>
@@ -3422,7 +3422,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C70" t="s">
         <v>142</v>
@@ -3448,7 +3448,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C71" t="s">
         <v>134</v>
@@ -3474,7 +3474,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C72" t="s">
         <v>132</v>
@@ -3500,7 +3500,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C73" t="s">
         <v>138</v>
@@ -3526,7 +3526,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C74" t="s">
         <v>144</v>
@@ -3556,7 +3556,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C75" t="s">
         <v>147</v>
@@ -3586,7 +3586,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C76" t="s">
         <v>149</v>
@@ -3616,7 +3616,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C77" t="s">
         <v>151</v>
@@ -3646,7 +3646,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C78" t="s">
         <v>153</v>
@@ -3676,7 +3676,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C79" t="s">
         <v>155</v>
@@ -3706,7 +3706,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C80" t="s">
         <v>157</v>
@@ -3736,7 +3736,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C81" t="s">
         <v>159</v>
@@ -3766,7 +3766,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C82" t="s">
         <v>161</v>
@@ -3796,7 +3796,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C83" t="s">
         <v>163</v>
@@ -3826,7 +3826,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C84" t="s">
         <v>165</v>
@@ -3856,7 +3856,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C85" t="s">
         <v>167</v>
@@ -3886,7 +3886,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C86" t="s">
         <v>169</v>
@@ -3916,7 +3916,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C87" t="s">
         <v>171</v>
@@ -3946,7 +3946,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C88" t="s">
         <v>173</v>
@@ -3976,7 +3976,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C89" t="s">
         <v>175</v>
@@ -4006,7 +4006,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C90" t="s">
         <v>146</v>
@@ -4061,13 +4061,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4434,8 +4434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{370C69D5-2497-4046-8AB5-D3D451AD9898}">
   <dimension ref="B3:AG22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AF8" sqref="AF8:AG19"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AN18" sqref="AN18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4449,7 +4449,7 @@
   <sheetData>
     <row r="3" spans="2:33" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>204</v>
+        <v>318</v>
       </c>
       <c r="AE3" s="2"/>
     </row>
@@ -5863,15 +5863,15 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" t="s">
         <v>205</v>
-      </c>
-      <c r="D1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -5882,7 +5882,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5893,7 +5893,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -5904,7 +5904,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5926,7 +5926,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B7" s="22">
         <v>0.21</v>
@@ -5937,7 +5937,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B8" s="22">
         <v>0.44</v>
@@ -5948,7 +5948,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B9" s="22">
         <v>0.64</v>
@@ -5959,7 +5959,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B10" s="22">
         <v>0.7</v>
@@ -5970,7 +5970,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B11" s="22">
         <v>0.81</v>
@@ -5981,7 +5981,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B12" s="22">
         <v>1.01</v>
@@ -5992,7 +5992,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B13" s="22">
         <v>1.56</v>
@@ -6003,7 +6003,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B14" s="22">
         <v>1.66</v>
@@ -6014,7 +6014,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B15" s="22">
         <v>1.83</v>
@@ -6025,7 +6025,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B16" s="22">
         <v>2.08</v>
@@ -6036,7 +6036,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B17" s="22">
         <v>2.1</v>
@@ -6047,7 +6047,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B18" s="22">
         <v>3.37</v>
@@ -6058,7 +6058,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B19" s="22">
         <v>3.5</v>
@@ -6069,7 +6069,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B20" s="22">
         <v>3.83</v>
@@ -6080,7 +6080,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B21" s="22">
         <v>4.01</v>
@@ -6091,7 +6091,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B22" s="22">
         <v>4.12</v>
@@ -6102,7 +6102,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B23" s="22">
         <v>4.95</v>
@@ -6113,7 +6113,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B24" s="22">
         <v>4.96</v>
@@ -6124,7 +6124,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B25" s="22">
         <v>5.22</v>
@@ -6135,7 +6135,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B26" s="22">
         <v>5.33</v>
@@ -6146,7 +6146,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B27" s="22">
         <v>5.52</v>
@@ -6157,7 +6157,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B28" s="22">
         <v>5.58</v>
@@ -6168,7 +6168,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B29" s="22">
         <v>5.97</v>
@@ -6179,7 +6179,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B30">
         <v>7.17</v>
@@ -6190,7 +6190,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B31">
         <v>7.2</v>
@@ -6201,7 +6201,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B32">
         <v>7.42</v>
@@ -6212,7 +6212,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B33">
         <v>7.49</v>
@@ -6223,7 +6223,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B34">
         <v>7.88</v>
@@ -6234,7 +6234,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B35">
         <v>7.99</v>
@@ -6245,7 +6245,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B36" s="21">
         <v>9.09</v>
@@ -6254,12 +6254,12 @@
         <v>100</v>
       </c>
       <c r="D36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B37" s="21">
         <v>10</v>
@@ -6268,12 +6268,12 @@
         <v>100</v>
       </c>
       <c r="D37" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B38">
         <v>10.26</v>
@@ -6284,7 +6284,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B39">
         <v>10.38</v>
@@ -6295,7 +6295,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B40" s="21">
         <v>10.6</v>
@@ -6304,12 +6304,12 @@
         <v>100</v>
       </c>
       <c r="D40" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B41">
         <v>11.15</v>
@@ -6320,7 +6320,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B42">
         <v>14.16</v>
@@ -6331,7 +6331,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B43" s="21">
         <v>17.149999999999999</v>
@@ -6340,12 +6340,12 @@
         <v>100</v>
       </c>
       <c r="D43" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B44">
         <v>17.5</v>
@@ -6356,7 +6356,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B45" s="21">
         <v>18.32</v>
@@ -6365,12 +6365,12 @@
         <v>100</v>
       </c>
       <c r="D45" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B46" s="21">
         <v>18.73</v>
@@ -6379,12 +6379,12 @@
         <v>100</v>
       </c>
       <c r="D46" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B47">
         <v>18.940000000000001</v>
@@ -6395,7 +6395,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B48">
         <v>19.05</v>
@@ -6406,7 +6406,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B49">
         <v>21.67</v>
@@ -6417,7 +6417,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B50">
         <v>21.8</v>
@@ -6428,7 +6428,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B51">
         <v>23.82</v>
@@ -6439,7 +6439,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B52">
         <v>25.36</v>
@@ -6450,7 +6450,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B53" s="21">
         <v>26.51</v>
@@ -6459,12 +6459,12 @@
         <v>100</v>
       </c>
       <c r="D53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B54" s="21">
         <v>27.47</v>
@@ -6473,12 +6473,12 @@
         <v>100</v>
       </c>
       <c r="D54" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B55">
         <v>27.72</v>
@@ -6489,7 +6489,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B56">
         <v>28.77</v>
@@ -6500,7 +6500,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B57" s="21">
         <v>29.07</v>
@@ -6509,12 +6509,12 @@
         <v>100</v>
       </c>
       <c r="D57" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B58">
         <v>29.16</v>
@@ -6525,7 +6525,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B59" s="21">
         <v>29.74</v>
@@ -6534,12 +6534,12 @@
         <v>100</v>
       </c>
       <c r="D59" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B60" s="21">
         <v>31.36</v>
@@ -6548,12 +6548,12 @@
         <v>100</v>
       </c>
       <c r="D60" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B61" s="21">
         <v>33.020000000000003</v>
@@ -6562,12 +6562,12 @@
         <v>100</v>
       </c>
       <c r="D61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B62" s="21">
         <v>35.31</v>
@@ -6576,12 +6576,12 @@
         <v>100</v>
       </c>
       <c r="D62" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B63" s="21">
         <v>37.33</v>
@@ -6590,12 +6590,12 @@
         <v>100</v>
       </c>
       <c r="D63" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B64" s="21">
         <v>40.58</v>
@@ -6604,12 +6604,12 @@
         <v>100</v>
       </c>
       <c r="D64" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B65" s="21">
         <v>42.4</v>
@@ -6618,12 +6618,12 @@
         <v>100</v>
       </c>
       <c r="D65" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B66" s="21">
         <v>42.79</v>
@@ -6632,12 +6632,12 @@
         <v>100</v>
       </c>
       <c r="D66" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B67">
         <v>45.72</v>
@@ -6648,7 +6648,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B68">
         <v>46.84</v>
@@ -6659,7 +6659,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B69" s="21">
         <v>47.45</v>
@@ -6668,12 +6668,12 @@
         <v>90</v>
       </c>
       <c r="D69" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B70" s="21">
         <v>48.04</v>
@@ -6682,12 +6682,12 @@
         <v>100</v>
       </c>
       <c r="D70" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B71" s="21">
         <v>53.38</v>
@@ -6696,12 +6696,12 @@
         <v>100</v>
       </c>
       <c r="D71" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B72" s="21">
         <v>53.46</v>
@@ -6710,12 +6710,12 @@
         <v>100</v>
       </c>
       <c r="D72" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B73" s="21">
         <v>53.77</v>
@@ -6724,12 +6724,12 @@
         <v>100</v>
       </c>
       <c r="D73" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B74" s="21">
         <v>57.13</v>
@@ -6738,12 +6738,12 @@
         <v>100</v>
       </c>
       <c r="D74" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B75" s="21">
         <v>58.49</v>
@@ -6752,12 +6752,12 @@
         <v>90</v>
       </c>
       <c r="D75" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B76" s="21">
         <v>61.54</v>
@@ -6766,12 +6766,12 @@
         <v>100</v>
       </c>
       <c r="D76" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B77" s="21">
         <v>67.430000000000007</v>
@@ -6780,12 +6780,12 @@
         <v>100</v>
       </c>
       <c r="D77" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B78" s="21">
         <v>68.900000000000006</v>
@@ -6794,12 +6794,12 @@
         <v>90</v>
       </c>
       <c r="D78" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B79" s="21">
         <v>72.319999999999993</v>
@@ -6808,12 +6808,12 @@
         <v>100</v>
       </c>
       <c r="D79" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B80" s="21">
         <v>81.66</v>
@@ -6822,12 +6822,12 @@
         <v>100</v>
       </c>
       <c r="D80" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B81" s="21">
         <v>83.68</v>
@@ -6836,7 +6836,7 @@
         <v>100</v>
       </c>
       <c r="D81" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -6850,7 +6850,7 @@
         <v>100</v>
       </c>
       <c r="D82" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -6864,7 +6864,7 @@
         <v>100</v>
       </c>
       <c r="D83" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -6878,7 +6878,7 @@
         <v>100</v>
       </c>
       <c r="D84" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -6892,7 +6892,7 @@
         <v>100</v>
       </c>
       <c r="D85" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -6906,7 +6906,7 @@
         <v>100</v>
       </c>
       <c r="D86" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -6920,7 +6920,7 @@
         <v>100</v>
       </c>
       <c r="D87" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -6934,7 +6934,7 @@
         <v>100</v>
       </c>
       <c r="D88" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -6948,7 +6948,7 @@
         <v>100</v>
       </c>
       <c r="D89" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -6962,7 +6962,7 @@
         <v>100</v>
       </c>
       <c r="D90" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -6976,7 +6976,7 @@
         <v>100</v>
       </c>
       <c r="D91" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -6990,7 +6990,7 @@
         <v>100</v>
       </c>
       <c r="D92" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -7004,7 +7004,7 @@
         <v>100</v>
       </c>
       <c r="D93" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -7018,7 +7018,7 @@
         <v>100</v>
       </c>
       <c r="D94" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -7032,7 +7032,7 @@
         <v>100</v>
       </c>
       <c r="D95" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -7046,7 +7046,7 @@
         <v>100</v>
       </c>
       <c r="D96" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -7060,7 +7060,7 @@
         <v>100</v>
       </c>
       <c r="D97" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -7101,60 +7101,60 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D1" t="s">
         <v>292</v>
       </c>
-      <c r="B1" t="s">
-        <v>289</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1" t="s">
+        <v>296</v>
+      </c>
+      <c r="I1" t="s">
+        <v>287</v>
+      </c>
+      <c r="J1" t="s">
+        <v>297</v>
+      </c>
+      <c r="K1" t="s">
+        <v>298</v>
+      </c>
+      <c r="L1" t="s">
+        <v>299</v>
+      </c>
+      <c r="M1" t="s">
         <v>290</v>
       </c>
-      <c r="D1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E1" t="s">
-        <v>294</v>
-      </c>
-      <c r="F1" t="s">
-        <v>295</v>
-      </c>
-      <c r="G1" t="s">
-        <v>296</v>
-      </c>
-      <c r="H1" t="s">
-        <v>297</v>
-      </c>
-      <c r="I1" t="s">
-        <v>288</v>
-      </c>
-      <c r="J1" t="s">
-        <v>298</v>
-      </c>
-      <c r="K1" t="s">
-        <v>299</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>300</v>
       </c>
-      <c r="M1" t="s">
-        <v>291</v>
-      </c>
-      <c r="N1" t="s">
-        <v>301</v>
-      </c>
       <c r="O1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="P1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>177</v>
@@ -7179,7 +7179,7 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J2" s="25">
         <v>60</v>
@@ -7251,12 +7251,12 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B20">
         <f>72*2</f>
@@ -7265,7 +7265,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B21">
         <f>16*2</f>
@@ -7274,7 +7274,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B22">
         <f>8*2</f>
@@ -7283,7 +7283,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B23">
         <f>SUM(B20:B22)</f>
@@ -7340,16 +7340,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7357,7 +7357,7 @@
         <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -7371,7 +7371,7 @@
         <v>177</v>
       </c>
       <c r="B3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -7385,7 +7385,7 @@
         <v>177</v>
       </c>
       <c r="B4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C4">
         <v>6</v>
@@ -7399,7 +7399,7 @@
         <v>177</v>
       </c>
       <c r="B5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -7413,7 +7413,7 @@
         <v>177</v>
       </c>
       <c r="B6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -7427,7 +7427,7 @@
         <v>177</v>
       </c>
       <c r="B7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -7441,7 +7441,7 @@
         <v>177</v>
       </c>
       <c r="B8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -7455,7 +7455,7 @@
         <v>177</v>
       </c>
       <c r="B9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -7469,7 +7469,7 @@
         <v>177</v>
       </c>
       <c r="B10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C10">
         <v>6</v>
@@ -7483,7 +7483,7 @@
         <v>177</v>
       </c>
       <c r="B11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C11">
         <v>6</v>
@@ -7497,7 +7497,7 @@
         <v>177</v>
       </c>
       <c r="B12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C12">
         <v>6</v>
@@ -7511,7 +7511,7 @@
         <v>177</v>
       </c>
       <c r="B13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C13">
         <v>6</v>
@@ -7525,7 +7525,7 @@
         <v>177</v>
       </c>
       <c r="B14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C14">
         <v>6</v>
@@ -7539,7 +7539,7 @@
         <v>177</v>
       </c>
       <c r="B15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C15">
         <v>6</v>
@@ -7553,7 +7553,7 @@
         <v>177</v>
       </c>
       <c r="B16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -7567,7 +7567,7 @@
         <v>177</v>
       </c>
       <c r="B17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -7581,7 +7581,7 @@
         <v>177</v>
       </c>
       <c r="B18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -7595,7 +7595,7 @@
         <v>177</v>
       </c>
       <c r="B19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C19">
         <v>6</v>
@@ -7609,7 +7609,7 @@
         <v>177</v>
       </c>
       <c r="B20" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C20">
         <v>6</v>
@@ -7623,7 +7623,7 @@
         <v>177</v>
       </c>
       <c r="B21" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C21">
         <v>6</v>
@@ -7637,7 +7637,7 @@
         <v>177</v>
       </c>
       <c r="B22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C22">
         <v>6</v>
@@ -7651,7 +7651,7 @@
         <v>177</v>
       </c>
       <c r="B23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C23">
         <v>6</v>
@@ -7665,7 +7665,7 @@
         <v>177</v>
       </c>
       <c r="B24" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C24">
         <v>6</v>
@@ -7679,7 +7679,7 @@
         <v>177</v>
       </c>
       <c r="B25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C25">
         <v>6</v>
@@ -7693,7 +7693,7 @@
         <v>177</v>
       </c>
       <c r="B26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C26">
         <v>6</v>
@@ -7707,7 +7707,7 @@
         <v>177</v>
       </c>
       <c r="B27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C27">
         <v>6</v>
@@ -7721,7 +7721,7 @@
         <v>177</v>
       </c>
       <c r="B28" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C28">
         <v>6</v>
@@ -7735,7 +7735,7 @@
         <v>177</v>
       </c>
       <c r="B29" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C29">
         <v>6</v>
@@ -7749,7 +7749,7 @@
         <v>177</v>
       </c>
       <c r="B30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C30">
         <v>6</v>
@@ -7763,7 +7763,7 @@
         <v>177</v>
       </c>
       <c r="B31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C31">
         <v>6</v>
@@ -7777,7 +7777,7 @@
         <v>177</v>
       </c>
       <c r="B32" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C32">
         <v>6</v>
@@ -7791,7 +7791,7 @@
         <v>177</v>
       </c>
       <c r="B33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C33">
         <v>6</v>

</xml_diff>

<commit_message>
seed lots for wubi
</commit_message>
<xml_diff>
--- a/data/planning.xlsx
+++ b/data/planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pth7\Documents\Intercrop JLJ\2025_winter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02F7A79-5974-464E-914C-8BC8A9C224D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2E4710-A13B-4FBE-9CEE-479665416E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="375" yWindow="240" windowWidth="31410" windowHeight="19080" xr2:uid="{BEFE39CF-4712-4775-9411-5C503787578E}"/>
   </bookViews>
@@ -2653,7 +2653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E147DB-166A-44B5-BCC5-098A0311CA8B}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
       <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>

</xml_diff>